<commit_message>
new stats with KO%
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxrak/Ricerca/measurement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxrak/Ricerca/LDSscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0DD321-21DA-4F43-868F-8266415E0CE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB97CE9-123A-834B-8972-6971C7F0E5AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320" activeTab="1" xr2:uid="{2AEA7D1B-2B5A-9B43-AAF2-E5A22E6D70D0}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -1146,7 +1146,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Dati!$C$151:$C$175</c:f>
+              <c:f>Dati!$C$226:$C$250</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1230,84 +1230,84 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Dati!$E$151:$E$175</c:f>
+              <c:f>Dati!$E$226:$E$250</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>148</c:v>
+                  <c:v>551</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>194</c:v>
+                  <c:v>1075</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>206</c:v>
+                  <c:v>1688</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>222</c:v>
+                  <c:v>2429</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>356</c:v>
+                  <c:v>2796</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>504</c:v>
+                  <c:v>3346</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>605</c:v>
+                  <c:v>3484</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>792</c:v>
+                  <c:v>3624</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>973</c:v>
+                  <c:v>4310</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1195</c:v>
+                  <c:v>4207</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1494</c:v>
+                  <c:v>4698</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1752</c:v>
+                  <c:v>5076</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1934</c:v>
+                  <c:v>5328</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2137</c:v>
+                  <c:v>4937</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2417</c:v>
+                  <c:v>5860</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2587</c:v>
+                  <c:v>5291</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2544</c:v>
+                  <c:v>6861</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2513</c:v>
+                  <c:v>6538</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2577</c:v>
+                  <c:v>6119</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2685</c:v>
+                  <c:v>6854</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2673</c:v>
+                  <c:v>6372</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2726</c:v>
+                  <c:v>6811</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2864</c:v>
+                  <c:v>7102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17409,8 +17409,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>41272</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Conf">
@@ -17433,7 +17433,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -20533,7 +20533,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D2E9F33D-B221-4049-99E8-5639C7C8CDB0}" name="Tabella pivot1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D2E9F33D-B221-4049-99E8-5639C7C8CDB0}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField dataField="1" showAll="0">
@@ -20939,7 +20939,7 @@
   <dimension ref="A1:H300"/>
   <sheetViews>
     <sheetView zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -29064,7 +29064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFE5CCF-2926-AE47-9614-07558948C5E6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>

</xml_diff>